<commit_message>
[EGSVC-30] Modified the asset category UI test
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/AssetCategoryDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/AssetCategoryDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="assetCategoryDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,16 +20,77 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">dataRow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assetCategoryType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parentCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deprecationMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assetAccountCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accumulatedDepreciationCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revaluationReserveAccountCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depreciationExpenceAccount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryDetails1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regExFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isActive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customFieldsDetails1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,8 +150,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -111,17 +176,64 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.6479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -137,20 +249,61 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.6479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>